<commit_message>
add db grid col table and dict
</commit_message>
<xml_diff>
--- a/db/busiui-dict.xlsx
+++ b/db/busiui-dict.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="296">
   <si>
     <t>静态数据字典StaticDataDictionary</t>
   </si>
@@ -924,14 +923,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>BUSIUI-form-支持绑定监听</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SYSAUTO022</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>onblur</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -945,6 +936,26 @@
   </si>
   <si>
     <t>onselect</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BUSIUI-事件类型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>校验</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义事件</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SYSAUTO023</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -952,7 +963,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1027,8 +1038,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1053,8 +1071,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1103,11 +1127,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1156,6 +1191,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1168,23 +1206,78 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="12"/>
+        <color rgb="FF9C0006"/>
+        <name val="宋体"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2044,28 +2137,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="12"/>
-        <color rgb="FF9C0006"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2366,10 +2437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I192"/>
+  <dimension ref="A1:K215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="F195" sqref="F195"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D187" sqref="D187:D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3081,17 +3152,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
     </row>
     <row r="2" spans="1:9" ht="24">
       <c r="A2" s="2" t="s">
@@ -3123,11 +3194,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="21" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="6">
@@ -3139,14 +3210,14 @@
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="21">
+      <c r="I3" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="6">
         <v>2</v>
       </c>
@@ -3156,12 +3227,12 @@
       <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
-      <c r="I4" s="21"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -3171,12 +3242,12 @@
       <c r="F5" s="8"/>
       <c r="G5" s="9"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="21"/>
+      <c r="I5" s="22"/>
     </row>
     <row r="6" spans="1:9" s="11" customFormat="1">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -3186,12 +3257,12 @@
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
       <c r="H6" s="10"/>
-      <c r="I6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" s="11" customFormat="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -3201,12 +3272,12 @@
       <c r="F7" s="12"/>
       <c r="G7" s="9"/>
       <c r="H7" s="10"/>
-      <c r="I7" s="21"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="6">
         <v>6</v>
       </c>
@@ -3216,12 +3287,12 @@
       <c r="F8" s="12"/>
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="21"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -3231,12 +3302,12 @@
       <c r="F9" s="12"/>
       <c r="G9" s="9"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -3246,12 +3317,12 @@
       <c r="F10" s="12"/>
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
-      <c r="I10" s="21"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="6">
         <v>9</v>
       </c>
@@ -3261,12 +3332,12 @@
       <c r="F11" s="12"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="21"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="6">
         <v>10</v>
       </c>
@@ -3276,12 +3347,12 @@
       <c r="F12" s="12"/>
       <c r="G12" s="9"/>
       <c r="H12" s="10"/>
-      <c r="I12" s="21"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="6">
         <v>11</v>
       </c>
@@ -3291,12 +3362,12 @@
       <c r="F13" s="12"/>
       <c r="G13" s="9"/>
       <c r="H13" s="10"/>
-      <c r="I13" s="21"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="6">
         <v>12</v>
       </c>
@@ -3306,12 +3377,12 @@
       <c r="F14" s="12"/>
       <c r="G14" s="9"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="21"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="6">
         <v>13</v>
       </c>
@@ -3321,12 +3392,12 @@
       <c r="F15" s="12"/>
       <c r="G15" s="9"/>
       <c r="H15" s="10"/>
-      <c r="I15" s="21"/>
+      <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="6">
         <v>14</v>
       </c>
@@ -3336,12 +3407,12 @@
       <c r="F16" s="12"/>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="21"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="6">
         <v>15</v>
       </c>
@@ -3351,12 +3422,12 @@
       <c r="F17" s="12"/>
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="21"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" s="11" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="6">
         <v>16</v>
       </c>
@@ -3366,12 +3437,12 @@
       <c r="F18" s="12"/>
       <c r="G18" s="9"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="21"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="6">
         <v>17</v>
       </c>
@@ -3381,12 +3452,12 @@
       <c r="F19" s="12"/>
       <c r="G19" s="9"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="21"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="6">
         <v>18</v>
       </c>
@@ -3399,9 +3470,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="6">
         <v>19</v>
       </c>
@@ -3414,9 +3485,9 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="11" customFormat="1">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="6">
         <v>20</v>
       </c>
@@ -3429,9 +3500,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" s="11" customFormat="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="6">
         <v>21</v>
       </c>
@@ -3444,11 +3515,11 @@
       <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" s="11" customFormat="1">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="6">
@@ -3460,14 +3531,14 @@
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="21">
+      <c r="I24" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="11" customFormat="1">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -3477,12 +3548,12 @@
       <c r="F25" s="8"/>
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="21"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" s="11" customFormat="1">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="6">
         <v>3</v>
       </c>
@@ -3492,12 +3563,12 @@
       <c r="F26" s="8"/>
       <c r="G26" s="9"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="21"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" s="11" customFormat="1">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="6">
         <v>4</v>
       </c>
@@ -3507,14 +3578,14 @@
       <c r="F27" s="8"/>
       <c r="G27" s="9"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="21"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" s="11" customFormat="1">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="21" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="6">
@@ -3526,14 +3597,14 @@
       <c r="F28" s="8"/>
       <c r="G28" s="9"/>
       <c r="H28" s="10"/>
-      <c r="I28" s="21">
+      <c r="I28" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="11" customFormat="1">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -3543,12 +3614,12 @@
       <c r="F29" s="8"/>
       <c r="G29" s="9"/>
       <c r="H29" s="10"/>
-      <c r="I29" s="21"/>
+      <c r="I29" s="22"/>
     </row>
     <row r="30" spans="1:9" s="11" customFormat="1">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="6">
         <v>3</v>
       </c>
@@ -3558,12 +3629,12 @@
       <c r="F30" s="8"/>
       <c r="G30" s="9"/>
       <c r="H30" s="10"/>
-      <c r="I30" s="21"/>
+      <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:9" s="11" customFormat="1">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="6">
         <v>4</v>
       </c>
@@ -3573,12 +3644,12 @@
       <c r="F31" s="8"/>
       <c r="G31" s="9"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="21"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" s="11" customFormat="1">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="6">
         <v>5</v>
       </c>
@@ -3588,12 +3659,12 @@
       <c r="F32" s="12"/>
       <c r="G32" s="9"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="21"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" s="11" customFormat="1">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="6">
         <v>6</v>
       </c>
@@ -3603,12 +3674,12 @@
       <c r="F33" s="12"/>
       <c r="G33" s="9"/>
       <c r="H33" s="10"/>
-      <c r="I33" s="21"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:9" s="11" customFormat="1">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="6">
         <v>7</v>
       </c>
@@ -3618,12 +3689,12 @@
       <c r="F34" s="12"/>
       <c r="G34" s="9"/>
       <c r="H34" s="10"/>
-      <c r="I34" s="21"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" s="11" customFormat="1">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="6">
         <v>8</v>
       </c>
@@ -3633,14 +3704,14 @@
       <c r="F35" s="12"/>
       <c r="G35" s="9"/>
       <c r="H35" s="10"/>
-      <c r="I35" s="21"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" s="11" customFormat="1">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="20"/>
+      <c r="C36" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="6">
@@ -3652,14 +3723,14 @@
       <c r="F36" s="8"/>
       <c r="G36" s="9"/>
       <c r="H36" s="10"/>
-      <c r="I36" s="21">
+      <c r="I36" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="11" customFormat="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="6">
         <v>2</v>
       </c>
@@ -3669,12 +3740,12 @@
       <c r="F37" s="8"/>
       <c r="G37" s="9"/>
       <c r="H37" s="10"/>
-      <c r="I37" s="21"/>
+      <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9" s="11" customFormat="1">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="6">
         <v>3</v>
       </c>
@@ -3684,12 +3755,12 @@
       <c r="F38" s="8"/>
       <c r="G38" s="9"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="21"/>
+      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" s="11" customFormat="1">
-      <c r="A39" s="18"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
       <c r="D39" s="6">
         <v>4</v>
       </c>
@@ -3699,12 +3770,12 @@
       <c r="F39" s="8"/>
       <c r="G39" s="9"/>
       <c r="H39" s="10"/>
-      <c r="I39" s="21"/>
+      <c r="I39" s="22"/>
     </row>
     <row r="40" spans="1:9" s="11" customFormat="1">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
       <c r="D40" s="6">
         <v>5</v>
       </c>
@@ -3714,12 +3785,12 @@
       <c r="F40" s="8"/>
       <c r="G40" s="9"/>
       <c r="H40" s="10"/>
-      <c r="I40" s="21"/>
+      <c r="I40" s="22"/>
     </row>
     <row r="41" spans="1:9" s="11" customFormat="1">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
       <c r="D41" s="6">
         <v>6</v>
       </c>
@@ -3729,14 +3800,14 @@
       <c r="F41" s="8"/>
       <c r="G41" s="9"/>
       <c r="H41" s="10"/>
-      <c r="I41" s="21"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" s="11" customFormat="1">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="20" t="s">
+      <c r="B42" s="20"/>
+      <c r="C42" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D42" s="6">
@@ -3748,14 +3819,14 @@
       <c r="F42" s="8"/>
       <c r="G42" s="9"/>
       <c r="H42" s="10"/>
-      <c r="I42" s="21">
+      <c r="I42" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="11" customFormat="1">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="6">
         <v>2</v>
       </c>
@@ -3765,12 +3836,12 @@
       <c r="F43" s="8"/>
       <c r="G43" s="9"/>
       <c r="H43" s="10"/>
-      <c r="I43" s="21"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" s="11" customFormat="1">
-      <c r="A44" s="18"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="6">
         <v>3</v>
       </c>
@@ -3780,12 +3851,12 @@
       <c r="F44" s="8"/>
       <c r="G44" s="9"/>
       <c r="H44" s="10"/>
-      <c r="I44" s="21"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" s="11" customFormat="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="6">
         <v>4</v>
       </c>
@@ -3795,12 +3866,12 @@
       <c r="F45" s="8"/>
       <c r="G45" s="9"/>
       <c r="H45" s="10"/>
-      <c r="I45" s="21"/>
+      <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:9" s="11" customFormat="1">
-      <c r="A46" s="18"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
       <c r="D46" s="6">
         <v>5</v>
       </c>
@@ -3810,12 +3881,12 @@
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
       <c r="H46" s="10"/>
-      <c r="I46" s="21"/>
+      <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:9" s="11" customFormat="1">
-      <c r="A47" s="18"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="6">
         <v>6</v>
       </c>
@@ -3825,14 +3896,14 @@
       <c r="F47" s="8"/>
       <c r="G47" s="9"/>
       <c r="H47" s="10"/>
-      <c r="I47" s="21"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" s="11" customFormat="1">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="20" t="s">
+      <c r="B48" s="20"/>
+      <c r="C48" s="21" t="s">
         <v>56</v>
       </c>
       <c r="D48" s="6">
@@ -3844,14 +3915,14 @@
       <c r="F48" s="8"/>
       <c r="G48" s="9"/>
       <c r="H48" s="10"/>
-      <c r="I48" s="21">
+      <c r="I48" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="11" customFormat="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="6">
         <v>4</v>
       </c>
@@ -3861,12 +3932,12 @@
       <c r="F49" s="8"/>
       <c r="G49" s="9"/>
       <c r="H49" s="10"/>
-      <c r="I49" s="21"/>
+      <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" s="11" customFormat="1">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="6">
         <v>5</v>
       </c>
@@ -3876,12 +3947,12 @@
       <c r="F50" s="8"/>
       <c r="G50" s="9"/>
       <c r="H50" s="10"/>
-      <c r="I50" s="21"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" s="11" customFormat="1">
-      <c r="A51" s="18"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="6">
         <v>6</v>
       </c>
@@ -3891,12 +3962,12 @@
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
       <c r="H51" s="10"/>
-      <c r="I51" s="21"/>
+      <c r="I51" s="22"/>
     </row>
     <row r="52" spans="1:9" s="11" customFormat="1">
-      <c r="A52" s="18"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="6">
         <v>7</v>
       </c>
@@ -3906,12 +3977,12 @@
       <c r="F52" s="8"/>
       <c r="G52" s="9"/>
       <c r="H52" s="10"/>
-      <c r="I52" s="21"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" s="11" customFormat="1">
-      <c r="A53" s="18"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="21"/>
       <c r="D53" s="6">
         <v>9</v>
       </c>
@@ -3921,12 +3992,12 @@
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="10"/>
-      <c r="I53" s="21"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" s="11" customFormat="1">
-      <c r="A54" s="18"/>
-      <c r="B54" s="19"/>
-      <c r="C54" s="20"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="6">
         <v>10</v>
       </c>
@@ -3936,12 +4007,12 @@
       <c r="F54" s="8"/>
       <c r="G54" s="9"/>
       <c r="H54" s="10"/>
-      <c r="I54" s="21"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" s="11" customFormat="1">
-      <c r="A55" s="18"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="20"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="6">
         <v>46</v>
       </c>
@@ -3951,12 +4022,12 @@
       <c r="F55" s="8"/>
       <c r="G55" s="9"/>
       <c r="H55" s="10"/>
-      <c r="I55" s="21"/>
+      <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" s="11" customFormat="1">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="6">
         <v>47</v>
       </c>
@@ -3966,12 +4037,12 @@
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
       <c r="H56" s="10"/>
-      <c r="I56" s="21"/>
+      <c r="I56" s="22"/>
     </row>
     <row r="57" spans="1:9" s="11" customFormat="1">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="6">
         <v>48</v>
       </c>
@@ -3981,12 +4052,12 @@
       <c r="F57" s="8"/>
       <c r="G57" s="9"/>
       <c r="H57" s="10"/>
-      <c r="I57" s="21"/>
+      <c r="I57" s="22"/>
     </row>
     <row r="58" spans="1:9" s="11" customFormat="1">
-      <c r="A58" s="18"/>
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="6">
         <v>49</v>
       </c>
@@ -3996,12 +4067,12 @@
       <c r="F58" s="8"/>
       <c r="G58" s="9"/>
       <c r="H58" s="10"/>
-      <c r="I58" s="21"/>
+      <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:9" s="11" customFormat="1">
-      <c r="A59" s="18"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
       <c r="D59" s="6">
         <v>50</v>
       </c>
@@ -4011,14 +4082,14 @@
       <c r="F59" s="8"/>
       <c r="G59" s="9"/>
       <c r="H59" s="10"/>
-      <c r="I59" s="21"/>
+      <c r="I59" s="22"/>
     </row>
     <row r="60" spans="1:9" s="11" customFormat="1">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="20" t="s">
+      <c r="B60" s="20"/>
+      <c r="C60" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D60" s="6">
@@ -4030,14 +4101,14 @@
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
       <c r="H60" s="10"/>
-      <c r="I60" s="21">
+      <c r="I60" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="11" customFormat="1">
-      <c r="A61" s="18"/>
-      <c r="B61" s="19"/>
-      <c r="C61" s="20"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="21"/>
       <c r="D61" s="6">
         <v>2</v>
       </c>
@@ -4047,12 +4118,12 @@
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
       <c r="H61" s="10"/>
-      <c r="I61" s="21"/>
+      <c r="I61" s="22"/>
     </row>
     <row r="62" spans="1:9" s="11" customFormat="1">
-      <c r="A62" s="18"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="21"/>
       <c r="D62" s="6">
         <v>3</v>
       </c>
@@ -4062,12 +4133,12 @@
       <c r="F62" s="8"/>
       <c r="G62" s="9"/>
       <c r="H62" s="10"/>
-      <c r="I62" s="21"/>
+      <c r="I62" s="22"/>
     </row>
     <row r="63" spans="1:9" s="11" customFormat="1">
-      <c r="A63" s="18"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="6">
         <v>4</v>
       </c>
@@ -4077,12 +4148,12 @@
       <c r="F63" s="8"/>
       <c r="G63" s="9"/>
       <c r="H63" s="10"/>
-      <c r="I63" s="21"/>
+      <c r="I63" s="22"/>
     </row>
     <row r="64" spans="1:9" s="11" customFormat="1">
-      <c r="A64" s="18"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="13">
         <v>5</v>
       </c>
@@ -4092,12 +4163,12 @@
       <c r="F64" s="8"/>
       <c r="G64" s="9"/>
       <c r="H64" s="10"/>
-      <c r="I64" s="21"/>
+      <c r="I64" s="22"/>
     </row>
     <row r="65" spans="1:9" s="11" customFormat="1">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
-      <c r="C65" s="20"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="21"/>
       <c r="D65" s="13">
         <v>6</v>
       </c>
@@ -4107,12 +4178,12 @@
       <c r="F65" s="8"/>
       <c r="G65" s="9"/>
       <c r="H65" s="10"/>
-      <c r="I65" s="21"/>
+      <c r="I65" s="22"/>
     </row>
     <row r="66" spans="1:9" s="11" customFormat="1">
-      <c r="A66" s="18"/>
-      <c r="B66" s="19"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="13">
         <v>7</v>
       </c>
@@ -4122,14 +4193,14 @@
       <c r="F66" s="8"/>
       <c r="G66" s="9"/>
       <c r="H66" s="10"/>
-      <c r="I66" s="21"/>
+      <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:9" s="11" customFormat="1">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="20" t="s">
+      <c r="B67" s="20"/>
+      <c r="C67" s="21" t="s">
         <v>79</v>
       </c>
       <c r="D67" s="6">
@@ -4141,14 +4212,14 @@
       <c r="F67" s="8"/>
       <c r="G67" s="9"/>
       <c r="H67" s="10"/>
-      <c r="I67" s="21">
+      <c r="I67" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="11" customFormat="1">
-      <c r="A68" s="18"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="21"/>
       <c r="D68" s="6">
         <v>2</v>
       </c>
@@ -4158,12 +4229,12 @@
       <c r="F68" s="8"/>
       <c r="G68" s="9"/>
       <c r="H68" s="10"/>
-      <c r="I68" s="21"/>
+      <c r="I68" s="22"/>
     </row>
     <row r="69" spans="1:9" s="11" customFormat="1">
-      <c r="A69" s="18"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="21"/>
       <c r="D69" s="6">
         <v>3</v>
       </c>
@@ -4173,14 +4244,14 @@
       <c r="F69" s="8"/>
       <c r="G69" s="9"/>
       <c r="H69" s="10"/>
-      <c r="I69" s="21"/>
+      <c r="I69" s="22"/>
     </row>
     <row r="70" spans="1:9" s="11" customFormat="1">
-      <c r="A70" s="18" t="s">
+      <c r="A70" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B70" s="19"/>
-      <c r="C70" s="20" t="s">
+      <c r="B70" s="20"/>
+      <c r="C70" s="21" t="s">
         <v>84</v>
       </c>
       <c r="D70" s="6">
@@ -4192,14 +4263,14 @@
       <c r="F70" s="8"/>
       <c r="G70" s="9"/>
       <c r="H70" s="10"/>
-      <c r="I70" s="21">
+      <c r="I70" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="11" customFormat="1">
-      <c r="A71" s="18"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="6">
         <v>2</v>
       </c>
@@ -4209,12 +4280,12 @@
       <c r="F71" s="8"/>
       <c r="G71" s="9"/>
       <c r="H71" s="10"/>
-      <c r="I71" s="21"/>
+      <c r="I71" s="22"/>
     </row>
     <row r="72" spans="1:9" s="11" customFormat="1">
-      <c r="A72" s="18"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="21"/>
       <c r="D72" s="6">
         <v>3</v>
       </c>
@@ -4224,12 +4295,12 @@
       <c r="F72" s="8"/>
       <c r="G72" s="9"/>
       <c r="H72" s="10"/>
-      <c r="I72" s="21"/>
+      <c r="I72" s="22"/>
     </row>
     <row r="73" spans="1:9" s="11" customFormat="1">
-      <c r="A73" s="18"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="21"/>
       <c r="D73" s="6">
         <v>4</v>
       </c>
@@ -4239,12 +4310,12 @@
       <c r="F73" s="8"/>
       <c r="G73" s="9"/>
       <c r="H73" s="10"/>
-      <c r="I73" s="21"/>
+      <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" s="11" customFormat="1">
-      <c r="A74" s="18"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="20"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="21"/>
       <c r="D74" s="6">
         <v>5</v>
       </c>
@@ -4254,14 +4325,14 @@
       <c r="F74" s="8"/>
       <c r="G74" s="9"/>
       <c r="H74" s="10"/>
-      <c r="I74" s="21"/>
+      <c r="I74" s="22"/>
     </row>
     <row r="75" spans="1:9" s="11" customFormat="1">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="20" t="s">
+      <c r="B75" s="20"/>
+      <c r="C75" s="21" t="s">
         <v>91</v>
       </c>
       <c r="D75" s="6">
@@ -4273,14 +4344,14 @@
       <c r="F75" s="8"/>
       <c r="G75" s="9"/>
       <c r="H75" s="10"/>
-      <c r="I75" s="21">
+      <c r="I75" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="11" customFormat="1">
-      <c r="A76" s="18"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="20"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="21"/>
       <c r="D76" s="6">
         <v>2</v>
       </c>
@@ -4290,12 +4361,12 @@
       <c r="F76" s="8"/>
       <c r="G76" s="9"/>
       <c r="H76" s="10"/>
-      <c r="I76" s="21"/>
+      <c r="I76" s="22"/>
     </row>
     <row r="77" spans="1:9" s="11" customFormat="1">
-      <c r="A77" s="18"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="20"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="21"/>
       <c r="D77" s="6">
         <v>3</v>
       </c>
@@ -4305,12 +4376,12 @@
       <c r="F77" s="8"/>
       <c r="G77" s="9"/>
       <c r="H77" s="10"/>
-      <c r="I77" s="21"/>
+      <c r="I77" s="22"/>
     </row>
     <row r="78" spans="1:9" s="11" customFormat="1">
-      <c r="A78" s="18"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="21"/>
       <c r="D78" s="6">
         <v>4</v>
       </c>
@@ -4320,12 +4391,12 @@
       <c r="F78" s="8"/>
       <c r="G78" s="9"/>
       <c r="H78" s="10"/>
-      <c r="I78" s="21"/>
+      <c r="I78" s="22"/>
     </row>
     <row r="79" spans="1:9" s="11" customFormat="1">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
+      <c r="A79" s="19"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="21"/>
       <c r="D79" s="6">
         <v>5</v>
       </c>
@@ -4335,12 +4406,12 @@
       <c r="F79" s="8"/>
       <c r="G79" s="9"/>
       <c r="H79" s="10"/>
-      <c r="I79" s="21"/>
+      <c r="I79" s="22"/>
     </row>
     <row r="80" spans="1:9" s="11" customFormat="1">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="19"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21"/>
       <c r="D80" s="6">
         <v>6</v>
       </c>
@@ -4350,12 +4421,12 @@
       <c r="F80" s="8"/>
       <c r="G80" s="9"/>
       <c r="H80" s="10"/>
-      <c r="I80" s="21"/>
+      <c r="I80" s="22"/>
     </row>
     <row r="81" spans="1:9" s="11" customFormat="1">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="20"/>
+      <c r="A81" s="19"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="21"/>
       <c r="D81" s="6">
         <v>7</v>
       </c>
@@ -4365,12 +4436,12 @@
       <c r="F81" s="8"/>
       <c r="G81" s="9"/>
       <c r="H81" s="10"/>
-      <c r="I81" s="21"/>
+      <c r="I81" s="22"/>
     </row>
     <row r="82" spans="1:9" s="11" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A82" s="18"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="20"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="21"/>
       <c r="D82" s="6">
         <v>8</v>
       </c>
@@ -4380,12 +4451,12 @@
       <c r="F82" s="8"/>
       <c r="G82" s="9"/>
       <c r="H82" s="10"/>
-      <c r="I82" s="21"/>
+      <c r="I82" s="22"/>
     </row>
     <row r="83" spans="1:9" s="11" customFormat="1">
-      <c r="A83" s="18"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="20"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="21"/>
       <c r="D83" s="6">
         <v>9</v>
       </c>
@@ -4398,9 +4469,9 @@
       <c r="I83" s="10"/>
     </row>
     <row r="84" spans="1:9" s="11" customFormat="1">
-      <c r="A84" s="18"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="20"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="21"/>
       <c r="D84" s="6">
         <v>10</v>
       </c>
@@ -4413,11 +4484,11 @@
       <c r="I84" s="10"/>
     </row>
     <row r="85" spans="1:9" s="11" customFormat="1">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B85" s="19"/>
-      <c r="C85" s="20" t="s">
+      <c r="B85" s="20"/>
+      <c r="C85" s="21" t="s">
         <v>103</v>
       </c>
       <c r="D85" s="6">
@@ -4429,14 +4500,14 @@
       <c r="F85" s="8"/>
       <c r="G85" s="9"/>
       <c r="H85" s="10"/>
-      <c r="I85" s="21">
+      <c r="I85" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="11" customFormat="1">
-      <c r="A86" s="18"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="20"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="21"/>
       <c r="D86" s="6">
         <v>20</v>
       </c>
@@ -4446,12 +4517,12 @@
       <c r="F86" s="8"/>
       <c r="G86" s="9"/>
       <c r="H86" s="10"/>
-      <c r="I86" s="21"/>
+      <c r="I86" s="22"/>
     </row>
     <row r="87" spans="1:9" s="11" customFormat="1" ht="15" customHeight="1">
-      <c r="A87" s="18"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="20"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="21"/>
       <c r="D87" s="6">
         <v>50</v>
       </c>
@@ -4461,12 +4532,12 @@
       <c r="F87" s="8"/>
       <c r="G87" s="9"/>
       <c r="H87" s="10"/>
-      <c r="I87" s="21"/>
+      <c r="I87" s="22"/>
     </row>
     <row r="88" spans="1:9" s="11" customFormat="1">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="20"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="21"/>
       <c r="D88" s="6">
         <v>100</v>
       </c>
@@ -4476,14 +4547,14 @@
       <c r="F88" s="8"/>
       <c r="G88" s="9"/>
       <c r="H88" s="10"/>
-      <c r="I88" s="21"/>
+      <c r="I88" s="22"/>
     </row>
     <row r="89" spans="1:9" s="11" customFormat="1">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B89" s="19"/>
-      <c r="C89" s="20" t="s">
+      <c r="B89" s="20"/>
+      <c r="C89" s="21" t="s">
         <v>105</v>
       </c>
       <c r="D89" s="6">
@@ -4495,14 +4566,14 @@
       <c r="F89" s="8"/>
       <c r="G89" s="9"/>
       <c r="H89" s="10"/>
-      <c r="I89" s="21">
+      <c r="I89" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="11" customFormat="1">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19"/>
-      <c r="C90" s="20"/>
+      <c r="A90" s="19"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="21"/>
       <c r="D90" s="6">
         <v>2</v>
       </c>
@@ -4512,12 +4583,12 @@
       <c r="F90" s="8"/>
       <c r="G90" s="9"/>
       <c r="H90" s="10"/>
-      <c r="I90" s="21"/>
+      <c r="I90" s="22"/>
     </row>
     <row r="91" spans="1:9" s="11" customFormat="1">
-      <c r="A91" s="18"/>
-      <c r="B91" s="19"/>
-      <c r="C91" s="20"/>
+      <c r="A91" s="19"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="21"/>
       <c r="D91" s="6">
         <v>3</v>
       </c>
@@ -4527,14 +4598,14 @@
       <c r="F91" s="8"/>
       <c r="G91" s="9"/>
       <c r="H91" s="10"/>
-      <c r="I91" s="21"/>
+      <c r="I91" s="22"/>
     </row>
     <row r="92" spans="1:9" s="11" customFormat="1">
-      <c r="A92" s="18" t="s">
+      <c r="A92" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="20" t="s">
+      <c r="B92" s="20"/>
+      <c r="C92" s="21" t="s">
         <v>109</v>
       </c>
       <c r="D92" s="6">
@@ -4546,14 +4617,14 @@
       <c r="F92" s="8"/>
       <c r="G92" s="9"/>
       <c r="H92" s="10"/>
-      <c r="I92" s="21">
+      <c r="I92" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:9" s="11" customFormat="1">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19"/>
-      <c r="C93" s="20"/>
+      <c r="A93" s="19"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="21"/>
       <c r="D93" s="6">
         <v>2</v>
       </c>
@@ -4563,14 +4634,14 @@
       <c r="F93" s="8"/>
       <c r="G93" s="9"/>
       <c r="H93" s="10"/>
-      <c r="I93" s="21"/>
+      <c r="I93" s="22"/>
     </row>
     <row r="94" spans="1:9" s="11" customFormat="1">
-      <c r="A94" s="18" t="s">
+      <c r="A94" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B94" s="19"/>
-      <c r="C94" s="20" t="s">
+      <c r="B94" s="20"/>
+      <c r="C94" s="21" t="s">
         <v>113</v>
       </c>
       <c r="D94" s="6">
@@ -4582,14 +4653,14 @@
       <c r="F94" s="8"/>
       <c r="G94" s="6"/>
       <c r="H94" s="10"/>
-      <c r="I94" s="21">
+      <c r="I94" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:9" s="11" customFormat="1">
-      <c r="A95" s="18"/>
-      <c r="B95" s="19"/>
-      <c r="C95" s="20"/>
+      <c r="A95" s="19"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="21"/>
       <c r="D95" s="6">
         <v>2</v>
       </c>
@@ -4599,12 +4670,12 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
       <c r="H95" s="10"/>
-      <c r="I95" s="21"/>
+      <c r="I95" s="22"/>
     </row>
     <row r="96" spans="1:9" s="11" customFormat="1">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19"/>
-      <c r="C96" s="20"/>
+      <c r="A96" s="19"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="21"/>
       <c r="D96" s="6">
         <v>3</v>
       </c>
@@ -4614,12 +4685,12 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
       <c r="H96" s="10"/>
-      <c r="I96" s="21"/>
+      <c r="I96" s="22"/>
     </row>
     <row r="97" spans="1:9" s="11" customFormat="1">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19"/>
-      <c r="C97" s="20"/>
+      <c r="A97" s="19"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="21"/>
       <c r="D97" s="6">
         <v>4</v>
       </c>
@@ -4629,12 +4700,12 @@
       <c r="F97" s="8"/>
       <c r="G97" s="9"/>
       <c r="H97" s="10"/>
-      <c r="I97" s="21"/>
+      <c r="I97" s="22"/>
     </row>
     <row r="98" spans="1:9" s="11" customFormat="1">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19"/>
-      <c r="C98" s="20"/>
+      <c r="A98" s="19"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="21"/>
       <c r="D98" s="6">
         <v>5</v>
       </c>
@@ -4644,12 +4715,12 @@
       <c r="F98" s="8"/>
       <c r="G98" s="9"/>
       <c r="H98" s="10"/>
-      <c r="I98" s="21"/>
+      <c r="I98" s="22"/>
     </row>
     <row r="99" spans="1:9" s="11" customFormat="1">
-      <c r="A99" s="18"/>
-      <c r="B99" s="19"/>
-      <c r="C99" s="20"/>
+      <c r="A99" s="19"/>
+      <c r="B99" s="20"/>
+      <c r="C99" s="21"/>
       <c r="D99" s="6">
         <v>6</v>
       </c>
@@ -4659,12 +4730,12 @@
       <c r="F99" s="8"/>
       <c r="G99" s="9"/>
       <c r="H99" s="10"/>
-      <c r="I99" s="21"/>
+      <c r="I99" s="22"/>
     </row>
     <row r="100" spans="1:9" s="11" customFormat="1">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19"/>
-      <c r="C100" s="20"/>
+      <c r="A100" s="19"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="21"/>
       <c r="D100" s="6">
         <v>7</v>
       </c>
@@ -4674,12 +4745,12 @@
       <c r="F100" s="8"/>
       <c r="G100" s="9"/>
       <c r="H100" s="10"/>
-      <c r="I100" s="21"/>
+      <c r="I100" s="22"/>
     </row>
     <row r="101" spans="1:9" s="11" customFormat="1">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19"/>
-      <c r="C101" s="20"/>
+      <c r="A101" s="19"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="21"/>
       <c r="D101" s="6">
         <v>8</v>
       </c>
@@ -4689,12 +4760,12 @@
       <c r="F101" s="8"/>
       <c r="G101" s="9"/>
       <c r="H101" s="10"/>
-      <c r="I101" s="21"/>
+      <c r="I101" s="22"/>
     </row>
     <row r="102" spans="1:9" s="11" customFormat="1">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19"/>
-      <c r="C102" s="20"/>
+      <c r="A102" s="19"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="21"/>
       <c r="D102" s="6">
         <v>9</v>
       </c>
@@ -4704,12 +4775,12 @@
       <c r="F102" s="8"/>
       <c r="G102" s="9"/>
       <c r="H102" s="10"/>
-      <c r="I102" s="21"/>
+      <c r="I102" s="22"/>
     </row>
     <row r="103" spans="1:9" s="11" customFormat="1">
-      <c r="A103" s="18"/>
-      <c r="B103" s="19"/>
-      <c r="C103" s="20"/>
+      <c r="A103" s="19"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="21"/>
       <c r="D103" s="6">
         <v>10</v>
       </c>
@@ -4719,12 +4790,12 @@
       <c r="F103" s="8"/>
       <c r="G103" s="9"/>
       <c r="H103" s="10"/>
-      <c r="I103" s="21"/>
+      <c r="I103" s="22"/>
     </row>
     <row r="104" spans="1:9" s="11" customFormat="1">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19"/>
-      <c r="C104" s="20"/>
+      <c r="A104" s="19"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="21"/>
       <c r="D104" s="6">
         <v>11</v>
       </c>
@@ -4734,12 +4805,12 @@
       <c r="F104" s="8"/>
       <c r="G104" s="9"/>
       <c r="H104" s="10"/>
-      <c r="I104" s="21"/>
+      <c r="I104" s="22"/>
     </row>
     <row r="105" spans="1:9" s="11" customFormat="1">
-      <c r="A105" s="18"/>
-      <c r="B105" s="19"/>
-      <c r="C105" s="20"/>
+      <c r="A105" s="19"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="21"/>
       <c r="D105" s="6">
         <v>12</v>
       </c>
@@ -4749,12 +4820,12 @@
       <c r="F105" s="8"/>
       <c r="G105" s="9"/>
       <c r="H105" s="10"/>
-      <c r="I105" s="21"/>
+      <c r="I105" s="22"/>
     </row>
     <row r="106" spans="1:9" s="11" customFormat="1">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19"/>
-      <c r="C106" s="20"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="21"/>
       <c r="D106" s="14">
         <v>13</v>
       </c>
@@ -4764,12 +4835,12 @@
       <c r="F106" s="8"/>
       <c r="G106" s="9"/>
       <c r="H106" s="10"/>
-      <c r="I106" s="21"/>
+      <c r="I106" s="22"/>
     </row>
     <row r="107" spans="1:9" s="11" customFormat="1">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19"/>
-      <c r="C107" s="20"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="21"/>
       <c r="D107" s="14">
         <v>14</v>
       </c>
@@ -4779,12 +4850,12 @@
       <c r="F107" s="8"/>
       <c r="G107" s="9"/>
       <c r="H107" s="10"/>
-      <c r="I107" s="21"/>
+      <c r="I107" s="22"/>
     </row>
     <row r="108" spans="1:9" s="11" customFormat="1">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19"/>
-      <c r="C108" s="20"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="21"/>
       <c r="D108" s="14">
         <v>15</v>
       </c>
@@ -4794,12 +4865,12 @@
       <c r="F108" s="8"/>
       <c r="G108" s="9"/>
       <c r="H108" s="10"/>
-      <c r="I108" s="21"/>
+      <c r="I108" s="22"/>
     </row>
     <row r="109" spans="1:9" s="11" customFormat="1">
-      <c r="A109" s="18"/>
-      <c r="B109" s="19"/>
-      <c r="C109" s="20"/>
+      <c r="A109" s="19"/>
+      <c r="B109" s="20"/>
+      <c r="C109" s="21"/>
       <c r="D109" s="6">
         <v>16</v>
       </c>
@@ -4809,12 +4880,12 @@
       <c r="F109" s="8"/>
       <c r="G109" s="9"/>
       <c r="H109" s="10"/>
-      <c r="I109" s="21"/>
+      <c r="I109" s="22"/>
     </row>
     <row r="110" spans="1:9" s="11" customFormat="1">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19"/>
-      <c r="C110" s="20"/>
+      <c r="A110" s="19"/>
+      <c r="B110" s="20"/>
+      <c r="C110" s="21"/>
       <c r="D110" s="6">
         <v>17</v>
       </c>
@@ -4824,14 +4895,14 @@
       <c r="F110" s="8"/>
       <c r="G110" s="9"/>
       <c r="H110" s="10"/>
-      <c r="I110" s="21"/>
+      <c r="I110" s="22"/>
     </row>
     <row r="111" spans="1:9" s="11" customFormat="1">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B111" s="19"/>
-      <c r="C111" s="20" t="s">
+      <c r="B111" s="20"/>
+      <c r="C111" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D111" s="6">
@@ -4843,14 +4914,14 @@
       <c r="F111" s="8"/>
       <c r="G111" s="9"/>
       <c r="H111" s="10"/>
-      <c r="I111" s="21">
+      <c r="I111" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="11" customFormat="1">
-      <c r="A112" s="18"/>
-      <c r="B112" s="19"/>
-      <c r="C112" s="20"/>
+      <c r="A112" s="19"/>
+      <c r="B112" s="20"/>
+      <c r="C112" s="21"/>
       <c r="D112" s="6">
         <v>2</v>
       </c>
@@ -4860,12 +4931,12 @@
       <c r="F112" s="8"/>
       <c r="G112" s="9"/>
       <c r="H112" s="10"/>
-      <c r="I112" s="21"/>
+      <c r="I112" s="22"/>
     </row>
     <row r="113" spans="1:9" s="11" customFormat="1">
-      <c r="A113" s="18"/>
-      <c r="B113" s="19"/>
-      <c r="C113" s="20"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="20"/>
+      <c r="C113" s="21"/>
       <c r="D113" s="6">
         <v>3</v>
       </c>
@@ -4875,14 +4946,14 @@
       <c r="F113" s="8"/>
       <c r="G113" s="9"/>
       <c r="H113" s="10"/>
-      <c r="I113" s="21"/>
+      <c r="I113" s="22"/>
     </row>
     <row r="114" spans="1:9" s="11" customFormat="1">
-      <c r="A114" s="20" t="s">
+      <c r="A114" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="20" t="s">
+      <c r="B114" s="20"/>
+      <c r="C114" s="21" t="s">
         <v>137</v>
       </c>
       <c r="D114" s="15">
@@ -4899,9 +4970,9 @@
       <c r="I114" s="10"/>
     </row>
     <row r="115" spans="1:9" s="11" customFormat="1">
-      <c r="A115" s="20"/>
-      <c r="B115" s="19"/>
-      <c r="C115" s="20"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="20"/>
+      <c r="C115" s="21"/>
       <c r="D115" s="6">
         <v>1</v>
       </c>
@@ -4913,14 +4984,14 @@
       </c>
       <c r="G115" s="9"/>
       <c r="H115" s="10"/>
-      <c r="I115" s="21">
+      <c r="I115" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="11" customFormat="1">
-      <c r="A116" s="20"/>
-      <c r="B116" s="19"/>
-      <c r="C116" s="20"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="21"/>
       <c r="D116" s="6">
         <v>2</v>
       </c>
@@ -4932,12 +5003,12 @@
       </c>
       <c r="G116" s="9"/>
       <c r="H116" s="10"/>
-      <c r="I116" s="21"/>
+      <c r="I116" s="22"/>
     </row>
     <row r="117" spans="1:9" s="11" customFormat="1">
-      <c r="A117" s="20"/>
-      <c r="B117" s="19"/>
-      <c r="C117" s="20"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="20"/>
+      <c r="C117" s="21"/>
       <c r="D117" s="6">
         <v>3</v>
       </c>
@@ -4949,12 +5020,12 @@
       </c>
       <c r="G117" s="9"/>
       <c r="H117" s="10"/>
-      <c r="I117" s="21"/>
+      <c r="I117" s="22"/>
     </row>
     <row r="118" spans="1:9" s="11" customFormat="1">
-      <c r="A118" s="20"/>
-      <c r="B118" s="19"/>
-      <c r="C118" s="20"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="21"/>
       <c r="D118" s="6">
         <v>4</v>
       </c>
@@ -4966,12 +5037,12 @@
       </c>
       <c r="G118" s="9"/>
       <c r="H118" s="10"/>
-      <c r="I118" s="21"/>
+      <c r="I118" s="22"/>
     </row>
     <row r="119" spans="1:9" s="11" customFormat="1">
-      <c r="A119" s="20"/>
-      <c r="B119" s="19"/>
-      <c r="C119" s="20"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="20"/>
+      <c r="C119" s="21"/>
       <c r="D119" s="6">
         <v>5</v>
       </c>
@@ -4983,12 +5054,12 @@
       </c>
       <c r="G119" s="9"/>
       <c r="H119" s="10"/>
-      <c r="I119" s="21"/>
+      <c r="I119" s="22"/>
     </row>
     <row r="120" spans="1:9" s="11" customFormat="1">
-      <c r="A120" s="20"/>
-      <c r="B120" s="19"/>
-      <c r="C120" s="20"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="21"/>
       <c r="D120" s="6">
         <v>6</v>
       </c>
@@ -5000,12 +5071,12 @@
       </c>
       <c r="G120" s="9"/>
       <c r="H120" s="10"/>
-      <c r="I120" s="21"/>
+      <c r="I120" s="22"/>
     </row>
     <row r="121" spans="1:9" s="11" customFormat="1">
-      <c r="A121" s="20"/>
-      <c r="B121" s="19"/>
-      <c r="C121" s="20"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="21"/>
       <c r="D121" s="6">
         <v>7</v>
       </c>
@@ -5017,12 +5088,12 @@
       </c>
       <c r="G121" s="9"/>
       <c r="H121" s="10"/>
-      <c r="I121" s="21"/>
+      <c r="I121" s="22"/>
     </row>
     <row r="122" spans="1:9" s="11" customFormat="1">
-      <c r="A122" s="20"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="20"/>
+      <c r="A122" s="21"/>
+      <c r="B122" s="20"/>
+      <c r="C122" s="21"/>
       <c r="D122" s="6">
         <v>8</v>
       </c>
@@ -5034,12 +5105,12 @@
       </c>
       <c r="G122" s="9"/>
       <c r="H122" s="10"/>
-      <c r="I122" s="21"/>
+      <c r="I122" s="22"/>
     </row>
     <row r="123" spans="1:9" s="11" customFormat="1">
-      <c r="A123" s="20"/>
-      <c r="B123" s="19"/>
-      <c r="C123" s="20"/>
+      <c r="A123" s="21"/>
+      <c r="B123" s="20"/>
+      <c r="C123" s="21"/>
       <c r="D123" s="6">
         <v>9</v>
       </c>
@@ -5051,12 +5122,12 @@
       </c>
       <c r="G123" s="9"/>
       <c r="H123" s="10"/>
-      <c r="I123" s="21"/>
+      <c r="I123" s="22"/>
     </row>
     <row r="124" spans="1:9" s="11" customFormat="1">
-      <c r="A124" s="20"/>
-      <c r="B124" s="19"/>
-      <c r="C124" s="20"/>
+      <c r="A124" s="21"/>
+      <c r="B124" s="20"/>
+      <c r="C124" s="21"/>
       <c r="D124" s="6">
         <v>10</v>
       </c>
@@ -5068,12 +5139,12 @@
       </c>
       <c r="G124" s="9"/>
       <c r="H124" s="10"/>
-      <c r="I124" s="21"/>
+      <c r="I124" s="22"/>
     </row>
     <row r="125" spans="1:9" s="11" customFormat="1">
-      <c r="A125" s="20"/>
-      <c r="B125" s="19"/>
-      <c r="C125" s="20"/>
+      <c r="A125" s="21"/>
+      <c r="B125" s="20"/>
+      <c r="C125" s="21"/>
       <c r="D125" s="6">
         <v>11</v>
       </c>
@@ -5085,12 +5156,12 @@
       </c>
       <c r="G125" s="9"/>
       <c r="H125" s="10"/>
-      <c r="I125" s="21"/>
+      <c r="I125" s="22"/>
     </row>
     <row r="126" spans="1:9" s="11" customFormat="1">
-      <c r="A126" s="20"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="20"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="20"/>
+      <c r="C126" s="21"/>
       <c r="D126" s="6">
         <v>12</v>
       </c>
@@ -5104,12 +5175,12 @@
         <v>164</v>
       </c>
       <c r="H126" s="10"/>
-      <c r="I126" s="21"/>
+      <c r="I126" s="22"/>
     </row>
     <row r="127" spans="1:9" s="11" customFormat="1">
-      <c r="A127" s="20"/>
-      <c r="B127" s="19"/>
-      <c r="C127" s="20"/>
+      <c r="A127" s="21"/>
+      <c r="B127" s="20"/>
+      <c r="C127" s="21"/>
       <c r="D127" s="6">
         <v>13</v>
       </c>
@@ -5123,12 +5194,12 @@
         <v>167</v>
       </c>
       <c r="H127" s="10"/>
-      <c r="I127" s="21"/>
+      <c r="I127" s="22"/>
     </row>
     <row r="128" spans="1:9" s="11" customFormat="1">
-      <c r="A128" s="20"/>
-      <c r="B128" s="19"/>
-      <c r="C128" s="20"/>
+      <c r="A128" s="21"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="21"/>
       <c r="D128" s="6">
         <v>14</v>
       </c>
@@ -5138,12 +5209,12 @@
       <c r="F128" s="6"/>
       <c r="G128" s="9"/>
       <c r="H128" s="10"/>
-      <c r="I128" s="21"/>
+      <c r="I128" s="22"/>
     </row>
     <row r="129" spans="1:9" s="11" customFormat="1">
-      <c r="A129" s="20"/>
-      <c r="B129" s="19"/>
-      <c r="C129" s="20"/>
+      <c r="A129" s="21"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="21"/>
       <c r="D129" s="6">
         <v>15</v>
       </c>
@@ -5153,12 +5224,12 @@
       <c r="F129" s="8"/>
       <c r="G129" s="9"/>
       <c r="H129" s="10"/>
-      <c r="I129" s="21"/>
+      <c r="I129" s="22"/>
     </row>
     <row r="130" spans="1:9" s="11" customFormat="1" ht="24">
-      <c r="A130" s="20"/>
-      <c r="B130" s="19"/>
-      <c r="C130" s="20"/>
+      <c r="A130" s="21"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="21"/>
       <c r="D130" s="6">
         <v>16</v>
       </c>
@@ -5170,12 +5241,12 @@
       </c>
       <c r="G130" s="9"/>
       <c r="H130" s="10"/>
-      <c r="I130" s="21"/>
+      <c r="I130" s="22"/>
     </row>
     <row r="131" spans="1:9" s="11" customFormat="1">
-      <c r="A131" s="20"/>
-      <c r="B131" s="19"/>
-      <c r="C131" s="20"/>
+      <c r="A131" s="21"/>
+      <c r="B131" s="20"/>
+      <c r="C131" s="21"/>
       <c r="D131" s="6">
         <v>17</v>
       </c>
@@ -5187,14 +5258,14 @@
       </c>
       <c r="G131" s="9"/>
       <c r="H131" s="10"/>
-      <c r="I131" s="21"/>
+      <c r="I131" s="22"/>
     </row>
     <row r="132" spans="1:9" s="11" customFormat="1">
-      <c r="A132" s="18" t="s">
+      <c r="A132" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B132" s="19"/>
-      <c r="C132" s="20" t="s">
+      <c r="B132" s="20"/>
+      <c r="C132" s="21" t="s">
         <v>175</v>
       </c>
       <c r="D132" s="6" t="s">
@@ -5206,14 +5277,14 @@
       <c r="F132" s="8"/>
       <c r="G132" s="9"/>
       <c r="H132" s="10"/>
-      <c r="I132" s="21">
+      <c r="I132" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:9" s="11" customFormat="1">
-      <c r="A133" s="18"/>
-      <c r="B133" s="19"/>
-      <c r="C133" s="20"/>
+      <c r="A133" s="19"/>
+      <c r="B133" s="20"/>
+      <c r="C133" s="21"/>
       <c r="D133" s="6" t="s">
         <v>178</v>
       </c>
@@ -5223,12 +5294,12 @@
       <c r="F133" s="8"/>
       <c r="G133" s="9"/>
       <c r="H133" s="10"/>
-      <c r="I133" s="21"/>
+      <c r="I133" s="22"/>
     </row>
     <row r="134" spans="1:9" s="11" customFormat="1">
-      <c r="A134" s="18"/>
-      <c r="B134" s="19"/>
-      <c r="C134" s="20"/>
+      <c r="A134" s="19"/>
+      <c r="B134" s="20"/>
+      <c r="C134" s="21"/>
       <c r="D134" s="6" t="s">
         <v>180</v>
       </c>
@@ -5238,12 +5309,12 @@
       <c r="F134" s="8"/>
       <c r="G134" s="9"/>
       <c r="H134" s="10"/>
-      <c r="I134" s="21"/>
+      <c r="I134" s="22"/>
     </row>
     <row r="135" spans="1:9" s="11" customFormat="1">
-      <c r="A135" s="18"/>
-      <c r="B135" s="19"/>
-      <c r="C135" s="20"/>
+      <c r="A135" s="19"/>
+      <c r="B135" s="20"/>
+      <c r="C135" s="21"/>
       <c r="D135" s="6" t="s">
         <v>182</v>
       </c>
@@ -5253,12 +5324,12 @@
       <c r="F135" s="8"/>
       <c r="G135" s="9"/>
       <c r="H135" s="10"/>
-      <c r="I135" s="21"/>
+      <c r="I135" s="22"/>
     </row>
     <row r="136" spans="1:9" s="11" customFormat="1">
-      <c r="A136" s="18"/>
-      <c r="B136" s="19"/>
-      <c r="C136" s="20"/>
+      <c r="A136" s="19"/>
+      <c r="B136" s="20"/>
+      <c r="C136" s="21"/>
       <c r="D136" s="6" t="s">
         <v>184</v>
       </c>
@@ -5268,12 +5339,12 @@
       <c r="F136" s="8"/>
       <c r="G136" s="9"/>
       <c r="H136" s="10"/>
-      <c r="I136" s="21"/>
+      <c r="I136" s="22"/>
     </row>
     <row r="137" spans="1:9" s="11" customFormat="1">
-      <c r="A137" s="18"/>
-      <c r="B137" s="19"/>
-      <c r="C137" s="20"/>
+      <c r="A137" s="19"/>
+      <c r="B137" s="20"/>
+      <c r="C137" s="21"/>
       <c r="D137" s="6" t="s">
         <v>186</v>
       </c>
@@ -5283,12 +5354,12 @@
       <c r="F137" s="8"/>
       <c r="G137" s="9"/>
       <c r="H137" s="10"/>
-      <c r="I137" s="21"/>
+      <c r="I137" s="22"/>
     </row>
     <row r="138" spans="1:9" s="11" customFormat="1">
-      <c r="A138" s="18"/>
-      <c r="B138" s="19"/>
-      <c r="C138" s="20"/>
+      <c r="A138" s="19"/>
+      <c r="B138" s="20"/>
+      <c r="C138" s="21"/>
       <c r="D138" s="6" t="s">
         <v>187</v>
       </c>
@@ -5302,12 +5373,12 @@
       <c r="H138" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="I138" s="21"/>
+      <c r="I138" s="22"/>
     </row>
     <row r="139" spans="1:9" s="11" customFormat="1">
-      <c r="A139" s="18"/>
-      <c r="B139" s="19"/>
-      <c r="C139" s="20"/>
+      <c r="A139" s="19"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="21"/>
       <c r="D139" s="6" t="s">
         <v>190</v>
       </c>
@@ -5321,12 +5392,12 @@
       <c r="H139" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="I139" s="21"/>
+      <c r="I139" s="22"/>
     </row>
     <row r="140" spans="1:9" s="11" customFormat="1">
-      <c r="A140" s="18"/>
-      <c r="B140" s="19"/>
-      <c r="C140" s="20"/>
+      <c r="A140" s="19"/>
+      <c r="B140" s="20"/>
+      <c r="C140" s="21"/>
       <c r="D140" s="6" t="s">
         <v>192</v>
       </c>
@@ -5340,12 +5411,12 @@
       <c r="H140" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="I140" s="21"/>
+      <c r="I140" s="22"/>
     </row>
     <row r="141" spans="1:9" s="11" customFormat="1">
-      <c r="A141" s="18"/>
-      <c r="B141" s="19"/>
-      <c r="C141" s="20"/>
+      <c r="A141" s="19"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="21"/>
       <c r="D141" s="6" t="s">
         <v>193</v>
       </c>
@@ -5359,12 +5430,12 @@
       <c r="H141" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="I141" s="21"/>
+      <c r="I141" s="22"/>
     </row>
     <row r="142" spans="1:9" s="11" customFormat="1">
-      <c r="A142" s="18"/>
-      <c r="B142" s="19"/>
-      <c r="C142" s="20"/>
+      <c r="A142" s="19"/>
+      <c r="B142" s="20"/>
+      <c r="C142" s="21"/>
       <c r="D142" s="6" t="s">
         <v>194</v>
       </c>
@@ -5378,12 +5449,12 @@
       <c r="H142" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="I142" s="21"/>
+      <c r="I142" s="22"/>
     </row>
     <row r="143" spans="1:9" s="11" customFormat="1">
-      <c r="A143" s="18"/>
-      <c r="B143" s="19"/>
-      <c r="C143" s="20"/>
+      <c r="A143" s="19"/>
+      <c r="B143" s="20"/>
+      <c r="C143" s="21"/>
       <c r="D143" s="6" t="s">
         <v>196</v>
       </c>
@@ -5397,12 +5468,12 @@
       <c r="H143" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="I143" s="21"/>
+      <c r="I143" s="22"/>
     </row>
     <row r="144" spans="1:9" s="11" customFormat="1">
-      <c r="A144" s="18"/>
-      <c r="B144" s="19"/>
-      <c r="C144" s="20"/>
+      <c r="A144" s="19"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="21"/>
       <c r="D144" s="6" t="s">
         <v>198</v>
       </c>
@@ -5416,12 +5487,12 @@
       <c r="H144" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="I144" s="21"/>
+      <c r="I144" s="22"/>
     </row>
     <row r="145" spans="1:9" s="11" customFormat="1">
-      <c r="A145" s="18"/>
-      <c r="B145" s="19"/>
-      <c r="C145" s="20"/>
+      <c r="A145" s="19"/>
+      <c r="B145" s="20"/>
+      <c r="C145" s="21"/>
       <c r="D145" s="6" t="s">
         <v>199</v>
       </c>
@@ -5435,12 +5506,12 @@
       <c r="H145" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="I145" s="21"/>
+      <c r="I145" s="22"/>
     </row>
     <row r="146" spans="1:9" s="11" customFormat="1">
-      <c r="A146" s="18"/>
-      <c r="B146" s="19"/>
-      <c r="C146" s="20"/>
+      <c r="A146" s="19"/>
+      <c r="B146" s="20"/>
+      <c r="C146" s="21"/>
       <c r="D146" s="6" t="s">
         <v>201</v>
       </c>
@@ -5454,12 +5525,12 @@
       <c r="H146" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="I146" s="21"/>
+      <c r="I146" s="22"/>
     </row>
     <row r="147" spans="1:9" s="11" customFormat="1">
-      <c r="A147" s="18"/>
-      <c r="B147" s="19"/>
-      <c r="C147" s="20"/>
+      <c r="A147" s="19"/>
+      <c r="B147" s="20"/>
+      <c r="C147" s="21"/>
       <c r="D147" s="6" t="s">
         <v>203</v>
       </c>
@@ -5473,12 +5544,12 @@
       <c r="H147" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="I147" s="21"/>
+      <c r="I147" s="22"/>
     </row>
     <row r="148" spans="1:9" s="11" customFormat="1">
-      <c r="A148" s="18"/>
-      <c r="B148" s="19"/>
-      <c r="C148" s="20"/>
+      <c r="A148" s="19"/>
+      <c r="B148" s="20"/>
+      <c r="C148" s="21"/>
       <c r="D148" s="6" t="s">
         <v>205</v>
       </c>
@@ -5492,12 +5563,12 @@
       <c r="H148" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="I148" s="21"/>
+      <c r="I148" s="22"/>
     </row>
     <row r="149" spans="1:9" s="11" customFormat="1">
-      <c r="A149" s="18"/>
-      <c r="B149" s="19"/>
-      <c r="C149" s="20"/>
+      <c r="A149" s="19"/>
+      <c r="B149" s="20"/>
+      <c r="C149" s="21"/>
       <c r="D149" s="6" t="s">
         <v>207</v>
       </c>
@@ -5511,12 +5582,12 @@
       <c r="H149" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="I149" s="21"/>
+      <c r="I149" s="22"/>
     </row>
     <row r="150" spans="1:9" s="11" customFormat="1">
-      <c r="A150" s="18"/>
-      <c r="B150" s="19"/>
-      <c r="C150" s="20"/>
+      <c r="A150" s="19"/>
+      <c r="B150" s="20"/>
+      <c r="C150" s="21"/>
       <c r="D150" s="6" t="s">
         <v>209</v>
       </c>
@@ -5530,12 +5601,12 @@
       <c r="H150" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="I150" s="21"/>
+      <c r="I150" s="22"/>
     </row>
     <row r="151" spans="1:9" s="11" customFormat="1">
-      <c r="A151" s="18"/>
-      <c r="B151" s="19"/>
-      <c r="C151" s="20"/>
+      <c r="A151" s="19"/>
+      <c r="B151" s="20"/>
+      <c r="C151" s="21"/>
       <c r="D151" s="6" t="s">
         <v>211</v>
       </c>
@@ -5549,12 +5620,12 @@
       <c r="H151" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="I151" s="21"/>
+      <c r="I151" s="22"/>
     </row>
     <row r="152" spans="1:9" s="11" customFormat="1">
-      <c r="A152" s="18"/>
-      <c r="B152" s="19"/>
-      <c r="C152" s="20"/>
+      <c r="A152" s="19"/>
+      <c r="B152" s="20"/>
+      <c r="C152" s="21"/>
       <c r="D152" s="6" t="s">
         <v>213</v>
       </c>
@@ -5568,12 +5639,12 @@
       <c r="H152" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="I152" s="21"/>
+      <c r="I152" s="22"/>
     </row>
     <row r="153" spans="1:9" s="11" customFormat="1">
-      <c r="A153" s="18"/>
-      <c r="B153" s="19"/>
-      <c r="C153" s="20"/>
+      <c r="A153" s="19"/>
+      <c r="B153" s="20"/>
+      <c r="C153" s="21"/>
       <c r="D153" s="6" t="s">
         <v>215</v>
       </c>
@@ -5587,12 +5658,12 @@
       <c r="H153" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="I153" s="21"/>
+      <c r="I153" s="22"/>
     </row>
     <row r="154" spans="1:9" s="11" customFormat="1">
-      <c r="A154" s="18"/>
-      <c r="B154" s="19"/>
-      <c r="C154" s="20"/>
+      <c r="A154" s="19"/>
+      <c r="B154" s="20"/>
+      <c r="C154" s="21"/>
       <c r="D154" s="6" t="s">
         <v>217</v>
       </c>
@@ -5606,12 +5677,12 @@
       <c r="H154" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="I154" s="21"/>
+      <c r="I154" s="22"/>
     </row>
     <row r="155" spans="1:9" s="11" customFormat="1">
-      <c r="A155" s="18"/>
-      <c r="B155" s="19"/>
-      <c r="C155" s="20"/>
+      <c r="A155" s="19"/>
+      <c r="B155" s="20"/>
+      <c r="C155" s="21"/>
       <c r="D155" s="6" t="s">
         <v>219</v>
       </c>
@@ -5625,12 +5696,12 @@
       <c r="H155" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="I155" s="21"/>
+      <c r="I155" s="22"/>
     </row>
     <row r="156" spans="1:9" s="11" customFormat="1">
-      <c r="A156" s="18"/>
-      <c r="B156" s="19"/>
-      <c r="C156" s="20"/>
+      <c r="A156" s="19"/>
+      <c r="B156" s="20"/>
+      <c r="C156" s="21"/>
       <c r="D156" s="6" t="s">
         <v>221</v>
       </c>
@@ -5644,12 +5715,12 @@
       <c r="H156" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="I156" s="21"/>
+      <c r="I156" s="22"/>
     </row>
     <row r="157" spans="1:9" s="11" customFormat="1">
-      <c r="A157" s="18"/>
-      <c r="B157" s="19"/>
-      <c r="C157" s="20"/>
+      <c r="A157" s="19"/>
+      <c r="B157" s="20"/>
+      <c r="C157" s="21"/>
       <c r="D157" s="6" t="s">
         <v>223</v>
       </c>
@@ -5663,12 +5734,12 @@
       <c r="H157" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="I157" s="21"/>
+      <c r="I157" s="22"/>
     </row>
     <row r="158" spans="1:9" s="11" customFormat="1">
-      <c r="A158" s="18"/>
-      <c r="B158" s="19"/>
-      <c r="C158" s="20"/>
+      <c r="A158" s="19"/>
+      <c r="B158" s="20"/>
+      <c r="C158" s="21"/>
       <c r="D158" s="6" t="s">
         <v>225</v>
       </c>
@@ -5682,12 +5753,12 @@
       <c r="H158" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="I158" s="21"/>
+      <c r="I158" s="22"/>
     </row>
     <row r="159" spans="1:9" s="11" customFormat="1">
-      <c r="A159" s="18"/>
-      <c r="B159" s="19"/>
-      <c r="C159" s="20"/>
+      <c r="A159" s="19"/>
+      <c r="B159" s="20"/>
+      <c r="C159" s="21"/>
       <c r="D159" s="6" t="s">
         <v>227</v>
       </c>
@@ -5701,12 +5772,12 @@
       <c r="H159" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="I159" s="21"/>
+      <c r="I159" s="22"/>
     </row>
     <row r="160" spans="1:9" s="11" customFormat="1">
-      <c r="A160" s="18"/>
-      <c r="B160" s="19"/>
-      <c r="C160" s="20"/>
+      <c r="A160" s="19"/>
+      <c r="B160" s="20"/>
+      <c r="C160" s="21"/>
       <c r="D160" s="6" t="s">
         <v>229</v>
       </c>
@@ -5720,12 +5791,12 @@
       <c r="H160" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="I160" s="21"/>
+      <c r="I160" s="22"/>
     </row>
     <row r="161" spans="1:9" s="11" customFormat="1">
-      <c r="A161" s="18"/>
-      <c r="B161" s="19"/>
-      <c r="C161" s="20"/>
+      <c r="A161" s="19"/>
+      <c r="B161" s="20"/>
+      <c r="C161" s="21"/>
       <c r="D161" s="6" t="s">
         <v>231</v>
       </c>
@@ -5739,12 +5810,12 @@
       <c r="H161" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="I161" s="21"/>
+      <c r="I161" s="22"/>
     </row>
     <row r="162" spans="1:9" s="11" customFormat="1">
-      <c r="A162" s="18"/>
-      <c r="B162" s="19"/>
-      <c r="C162" s="20"/>
+      <c r="A162" s="19"/>
+      <c r="B162" s="20"/>
+      <c r="C162" s="21"/>
       <c r="D162" s="6" t="s">
         <v>233</v>
       </c>
@@ -5758,12 +5829,12 @@
       <c r="H162" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="I162" s="21"/>
+      <c r="I162" s="22"/>
     </row>
     <row r="163" spans="1:9" s="11" customFormat="1">
-      <c r="A163" s="18"/>
-      <c r="B163" s="19"/>
-      <c r="C163" s="20"/>
+      <c r="A163" s="19"/>
+      <c r="B163" s="20"/>
+      <c r="C163" s="21"/>
       <c r="D163" s="6" t="s">
         <v>235</v>
       </c>
@@ -5777,12 +5848,12 @@
       <c r="H163" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="I163" s="21"/>
+      <c r="I163" s="22"/>
     </row>
     <row r="164" spans="1:9" s="11" customFormat="1">
-      <c r="A164" s="18"/>
-      <c r="B164" s="19"/>
-      <c r="C164" s="20"/>
+      <c r="A164" s="19"/>
+      <c r="B164" s="20"/>
+      <c r="C164" s="21"/>
       <c r="D164" s="6" t="s">
         <v>237</v>
       </c>
@@ -5796,12 +5867,12 @@
       <c r="H164" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I164" s="21"/>
+      <c r="I164" s="22"/>
     </row>
     <row r="165" spans="1:9" s="11" customFormat="1">
-      <c r="A165" s="18"/>
-      <c r="B165" s="19"/>
-      <c r="C165" s="20"/>
+      <c r="A165" s="19"/>
+      <c r="B165" s="20"/>
+      <c r="C165" s="21"/>
       <c r="D165" s="6" t="s">
         <v>239</v>
       </c>
@@ -5815,12 +5886,12 @@
       <c r="H165" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="I165" s="21"/>
+      <c r="I165" s="22"/>
     </row>
     <row r="166" spans="1:9" s="11" customFormat="1">
-      <c r="A166" s="18"/>
-      <c r="B166" s="19"/>
-      <c r="C166" s="20"/>
+      <c r="A166" s="19"/>
+      <c r="B166" s="20"/>
+      <c r="C166" s="21"/>
       <c r="D166" s="6" t="s">
         <v>241</v>
       </c>
@@ -5834,12 +5905,12 @@
       <c r="H166" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="I166" s="21"/>
+      <c r="I166" s="22"/>
     </row>
     <row r="167" spans="1:9" s="11" customFormat="1">
-      <c r="A167" s="18"/>
-      <c r="B167" s="19"/>
-      <c r="C167" s="20"/>
+      <c r="A167" s="19"/>
+      <c r="B167" s="20"/>
+      <c r="C167" s="21"/>
       <c r="D167" s="6" t="s">
         <v>243</v>
       </c>
@@ -5853,12 +5924,12 @@
       <c r="H167" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="I167" s="21"/>
+      <c r="I167" s="22"/>
     </row>
     <row r="168" spans="1:9" s="11" customFormat="1">
-      <c r="A168" s="18"/>
-      <c r="B168" s="19"/>
-      <c r="C168" s="20"/>
+      <c r="A168" s="19"/>
+      <c r="B168" s="20"/>
+      <c r="C168" s="21"/>
       <c r="D168" s="6" t="s">
         <v>245</v>
       </c>
@@ -5872,12 +5943,12 @@
       <c r="H168" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="I168" s="21"/>
+      <c r="I168" s="22"/>
     </row>
     <row r="169" spans="1:9" s="11" customFormat="1">
-      <c r="A169" s="18"/>
-      <c r="B169" s="19"/>
-      <c r="C169" s="20"/>
+      <c r="A169" s="19"/>
+      <c r="B169" s="20"/>
+      <c r="C169" s="21"/>
       <c r="D169" s="6" t="s">
         <v>247</v>
       </c>
@@ -5891,12 +5962,12 @@
       <c r="H169" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="I169" s="21"/>
+      <c r="I169" s="22"/>
     </row>
     <row r="170" spans="1:9" s="11" customFormat="1">
-      <c r="A170" s="18"/>
-      <c r="B170" s="19"/>
-      <c r="C170" s="20"/>
+      <c r="A170" s="19"/>
+      <c r="B170" s="20"/>
+      <c r="C170" s="21"/>
       <c r="D170" s="6" t="s">
         <v>249</v>
       </c>
@@ -5910,12 +5981,12 @@
       <c r="H170" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="I170" s="21"/>
+      <c r="I170" s="22"/>
     </row>
     <row r="171" spans="1:9" s="11" customFormat="1">
-      <c r="A171" s="18"/>
-      <c r="B171" s="19"/>
-      <c r="C171" s="20"/>
+      <c r="A171" s="19"/>
+      <c r="B171" s="20"/>
+      <c r="C171" s="21"/>
       <c r="D171" s="6" t="s">
         <v>251</v>
       </c>
@@ -5929,12 +6000,12 @@
       <c r="H171" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="I171" s="21"/>
+      <c r="I171" s="22"/>
     </row>
     <row r="172" spans="1:9" s="11" customFormat="1">
-      <c r="A172" s="18"/>
-      <c r="B172" s="19"/>
-      <c r="C172" s="20"/>
+      <c r="A172" s="19"/>
+      <c r="B172" s="20"/>
+      <c r="C172" s="21"/>
       <c r="D172" s="6" t="s">
         <v>253</v>
       </c>
@@ -5948,12 +6019,12 @@
       <c r="H172" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="I172" s="21"/>
+      <c r="I172" s="22"/>
     </row>
     <row r="173" spans="1:9" s="11" customFormat="1">
-      <c r="A173" s="18"/>
-      <c r="B173" s="19"/>
-      <c r="C173" s="20"/>
+      <c r="A173" s="19"/>
+      <c r="B173" s="20"/>
+      <c r="C173" s="21"/>
       <c r="D173" s="6" t="s">
         <v>255</v>
       </c>
@@ -5967,12 +6038,12 @@
       <c r="H173" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="I173" s="21"/>
+      <c r="I173" s="22"/>
     </row>
     <row r="174" spans="1:9" s="11" customFormat="1">
-      <c r="A174" s="18"/>
-      <c r="B174" s="19"/>
-      <c r="C174" s="20"/>
+      <c r="A174" s="19"/>
+      <c r="B174" s="20"/>
+      <c r="C174" s="21"/>
       <c r="D174" s="6" t="s">
         <v>257</v>
       </c>
@@ -5986,12 +6057,12 @@
       <c r="H174" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="I174" s="21"/>
+      <c r="I174" s="22"/>
     </row>
     <row r="175" spans="1:9" s="11" customFormat="1">
-      <c r="A175" s="18"/>
-      <c r="B175" s="19"/>
-      <c r="C175" s="20"/>
+      <c r="A175" s="19"/>
+      <c r="B175" s="20"/>
+      <c r="C175" s="21"/>
       <c r="D175" s="6" t="s">
         <v>259</v>
       </c>
@@ -6005,12 +6076,12 @@
       <c r="H175" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I175" s="21"/>
+      <c r="I175" s="22"/>
     </row>
     <row r="176" spans="1:9" s="11" customFormat="1">
-      <c r="A176" s="18"/>
-      <c r="B176" s="19"/>
-      <c r="C176" s="20"/>
+      <c r="A176" s="19"/>
+      <c r="B176" s="20"/>
+      <c r="C176" s="21"/>
       <c r="D176" s="6" t="s">
         <v>261</v>
       </c>
@@ -6024,12 +6095,12 @@
       <c r="H176" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="I176" s="21"/>
+      <c r="I176" s="22"/>
     </row>
     <row r="177" spans="1:9" s="11" customFormat="1">
-      <c r="A177" s="18"/>
-      <c r="B177" s="19"/>
-      <c r="C177" s="20"/>
+      <c r="A177" s="19"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="21"/>
       <c r="D177" s="6" t="s">
         <v>263</v>
       </c>
@@ -6043,12 +6114,12 @@
       <c r="H177" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="I177" s="21"/>
+      <c r="I177" s="22"/>
     </row>
     <row r="178" spans="1:9" s="11" customFormat="1">
-      <c r="A178" s="18"/>
-      <c r="B178" s="19"/>
-      <c r="C178" s="20"/>
+      <c r="A178" s="19"/>
+      <c r="B178" s="20"/>
+      <c r="C178" s="21"/>
       <c r="D178" s="6" t="s">
         <v>265</v>
       </c>
@@ -6062,12 +6133,12 @@
       <c r="H178" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="I178" s="21"/>
+      <c r="I178" s="22"/>
     </row>
     <row r="179" spans="1:9" s="11" customFormat="1">
-      <c r="A179" s="18"/>
-      <c r="B179" s="19"/>
-      <c r="C179" s="20"/>
+      <c r="A179" s="19"/>
+      <c r="B179" s="20"/>
+      <c r="C179" s="21"/>
       <c r="D179" s="6" t="s">
         <v>266</v>
       </c>
@@ -6081,14 +6152,14 @@
       <c r="H179" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="I179" s="21"/>
+      <c r="I179" s="22"/>
     </row>
     <row r="180" spans="1:9" s="11" customFormat="1">
-      <c r="A180" s="18" t="s">
+      <c r="A180" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="B180" s="19"/>
-      <c r="C180" s="20" t="s">
+      <c r="B180" s="20"/>
+      <c r="C180" s="21" t="s">
         <v>280</v>
       </c>
       <c r="D180" s="6">
@@ -6100,14 +6171,14 @@
       <c r="F180" s="8"/>
       <c r="G180" s="9"/>
       <c r="H180" s="10"/>
-      <c r="I180" s="24">
+      <c r="I180" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:9" s="11" customFormat="1">
-      <c r="A181" s="18"/>
-      <c r="B181" s="19"/>
-      <c r="C181" s="20"/>
+      <c r="A181" s="19"/>
+      <c r="B181" s="20"/>
+      <c r="C181" s="21"/>
       <c r="D181" s="6">
         <v>2</v>
       </c>
@@ -6117,14 +6188,14 @@
       <c r="F181" s="8"/>
       <c r="G181" s="9"/>
       <c r="H181" s="10"/>
-      <c r="I181" s="25"/>
+      <c r="I181" s="24"/>
     </row>
     <row r="182" spans="1:9" s="11" customFormat="1">
-      <c r="A182" s="18" t="s">
+      <c r="A182" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="B182" s="19"/>
-      <c r="C182" s="20" t="s">
+      <c r="B182" s="20"/>
+      <c r="C182" s="21" t="s">
         <v>272</v>
       </c>
       <c r="D182" s="6">
@@ -6136,14 +6207,14 @@
       <c r="F182" s="8"/>
       <c r="G182" s="9"/>
       <c r="H182" s="10"/>
-      <c r="I182" s="21">
+      <c r="I182" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:9" s="11" customFormat="1">
-      <c r="A183" s="18"/>
-      <c r="B183" s="19"/>
-      <c r="C183" s="20"/>
+      <c r="A183" s="19"/>
+      <c r="B183" s="20"/>
+      <c r="C183" s="21"/>
       <c r="D183" s="6">
         <v>1</v>
       </c>
@@ -6153,14 +6224,14 @@
       <c r="F183" s="8"/>
       <c r="G183" s="9"/>
       <c r="H183" s="10"/>
-      <c r="I183" s="21"/>
+      <c r="I183" s="22"/>
     </row>
     <row r="184" spans="1:9" s="11" customFormat="1">
-      <c r="A184" s="18" t="s">
+      <c r="A184" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="B184" s="19"/>
-      <c r="C184" s="20" t="s">
+      <c r="B184" s="20"/>
+      <c r="C184" s="21" t="s">
         <v>276</v>
       </c>
       <c r="D184" s="6">
@@ -6172,14 +6243,14 @@
       <c r="F184" s="8"/>
       <c r="G184" s="9"/>
       <c r="H184" s="10"/>
-      <c r="I184" s="21">
+      <c r="I184" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:9" s="11" customFormat="1">
-      <c r="A185" s="18"/>
-      <c r="B185" s="19"/>
-      <c r="C185" s="20"/>
+      <c r="A185" s="19"/>
+      <c r="B185" s="20"/>
+      <c r="C185" s="21"/>
       <c r="D185" s="6">
         <v>2</v>
       </c>
@@ -6189,12 +6260,12 @@
       <c r="F185" s="8"/>
       <c r="G185" s="9"/>
       <c r="H185" s="10"/>
-      <c r="I185" s="21"/>
+      <c r="I185" s="22"/>
     </row>
     <row r="186" spans="1:9" s="11" customFormat="1">
-      <c r="A186" s="18"/>
-      <c r="B186" s="19"/>
-      <c r="C186" s="20"/>
+      <c r="A186" s="19"/>
+      <c r="B186" s="20"/>
+      <c r="C186" s="21"/>
       <c r="D186" s="6">
         <v>3</v>
       </c>
@@ -6204,14 +6275,14 @@
       <c r="F186" s="8"/>
       <c r="G186" s="9"/>
       <c r="H186" s="10"/>
-      <c r="I186" s="21"/>
-    </row>
-    <row r="187" spans="1:9" s="11" customFormat="1">
-      <c r="A187" s="18" t="s">
+      <c r="I186" s="22"/>
+    </row>
+    <row r="187" spans="1:9" s="11" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A187" s="32" t="s">
         <v>284</v>
       </c>
-      <c r="B187" s="19"/>
-      <c r="C187" s="20" t="s">
+      <c r="B187" s="35"/>
+      <c r="C187" s="29" t="s">
         <v>283</v>
       </c>
       <c r="D187" s="6">
@@ -6223,14 +6294,14 @@
       <c r="F187" s="8"/>
       <c r="G187" s="9"/>
       <c r="H187" s="17"/>
-      <c r="I187" s="21">
+      <c r="I187" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:9" s="11" customFormat="1">
-      <c r="A188" s="18"/>
-      <c r="B188" s="19"/>
-      <c r="C188" s="20"/>
+      <c r="A188" s="33"/>
+      <c r="B188" s="36"/>
+      <c r="C188" s="30"/>
       <c r="D188" s="6">
         <v>2</v>
       </c>
@@ -6240,84 +6311,498 @@
       <c r="F188" s="8"/>
       <c r="G188" s="9"/>
       <c r="H188" s="17"/>
-      <c r="I188" s="21"/>
-    </row>
-    <row r="189" spans="1:9">
-      <c r="A189" s="18" t="s">
+      <c r="I188" s="22"/>
+    </row>
+    <row r="189" spans="1:9" ht="13.5" customHeight="1">
+      <c r="A189" s="33"/>
+      <c r="B189" s="36"/>
+      <c r="C189" s="30"/>
+      <c r="D189" s="6">
+        <v>3</v>
+      </c>
+      <c r="E189" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="B189" s="19"/>
-      <c r="C189" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="D189" s="6">
-        <v>1</v>
-      </c>
-      <c r="E189" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="F189" s="8"/>
       <c r="G189" s="9"/>
       <c r="H189" s="17"/>
-      <c r="I189" s="21">
+      <c r="I189" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:9">
-      <c r="A190" s="18"/>
-      <c r="B190" s="19"/>
-      <c r="C190" s="20"/>
+      <c r="A190" s="33"/>
+      <c r="B190" s="36"/>
+      <c r="C190" s="30"/>
       <c r="D190" s="6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F190" s="8"/>
       <c r="G190" s="9"/>
       <c r="H190" s="17"/>
-      <c r="I190" s="21"/>
+      <c r="I190" s="22"/>
     </row>
     <row r="191" spans="1:9">
-      <c r="A191" s="18"/>
-      <c r="B191" s="19"/>
-      <c r="C191" s="20"/>
+      <c r="A191" s="33"/>
+      <c r="B191" s="36"/>
+      <c r="C191" s="30"/>
       <c r="D191" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F191" s="8"/>
       <c r="G191" s="9"/>
       <c r="H191" s="17"/>
-      <c r="I191" s="21"/>
+      <c r="I191" s="22"/>
     </row>
     <row r="192" spans="1:9">
-      <c r="A192" s="18"/>
-      <c r="B192" s="19"/>
-      <c r="C192" s="20"/>
+      <c r="A192" s="34"/>
+      <c r="B192" s="37"/>
+      <c r="C192" s="31"/>
       <c r="D192" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F192" s="8"/>
       <c r="G192" s="9"/>
       <c r="H192" s="17"/>
-      <c r="I192" s="21"/>
+      <c r="I192" s="22"/>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="B193" s="20"/>
+      <c r="C193" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="D193" s="6">
+        <v>1</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F193" s="8"/>
+      <c r="G193" s="9"/>
+      <c r="H193" s="18"/>
+      <c r="I193" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
+      <c r="A194" s="19"/>
+      <c r="B194" s="20"/>
+      <c r="C194" s="21"/>
+      <c r="D194" s="6">
+        <v>2</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F194" s="8"/>
+      <c r="G194" s="9"/>
+      <c r="H194" s="18"/>
+      <c r="I194" s="22"/>
+    </row>
+    <row r="195" spans="1:11">
+      <c r="A195" s="19"/>
+      <c r="B195" s="20"/>
+      <c r="C195" s="21"/>
+      <c r="D195" s="6">
+        <v>3</v>
+      </c>
+      <c r="E195" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F195" s="8"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="18"/>
+      <c r="I195" s="22"/>
+    </row>
+    <row r="196" spans="1:11">
+      <c r="A196" s="19"/>
+      <c r="B196" s="20"/>
+      <c r="C196" s="21"/>
+      <c r="D196" s="6">
+        <v>4</v>
+      </c>
+      <c r="E196" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F196" s="8"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="18"/>
+      <c r="I196" s="22"/>
+    </row>
+    <row r="197" spans="1:11">
+      <c r="A197" s="19"/>
+      <c r="B197" s="20"/>
+      <c r="C197" s="21"/>
+      <c r="D197" s="6">
+        <v>5</v>
+      </c>
+      <c r="E197" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F197" s="8"/>
+      <c r="G197" s="9"/>
+      <c r="H197" s="18"/>
+      <c r="I197" s="22"/>
+    </row>
+    <row r="198" spans="1:11">
+      <c r="A198" s="19"/>
+      <c r="B198" s="20"/>
+      <c r="C198" s="21"/>
+      <c r="D198" s="6">
+        <v>6</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F198" s="8"/>
+      <c r="G198" s="9"/>
+      <c r="H198" s="18"/>
+      <c r="I198" s="22"/>
+    </row>
+    <row r="199" spans="1:11">
+      <c r="A199" s="19"/>
+      <c r="B199" s="20"/>
+      <c r="C199" s="21"/>
+      <c r="D199" s="6">
+        <v>7</v>
+      </c>
+      <c r="E199" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F199" s="8"/>
+      <c r="G199" s="9"/>
+      <c r="H199" s="18"/>
+      <c r="I199" s="22"/>
+    </row>
+    <row r="200" spans="1:11">
+      <c r="A200" s="19"/>
+      <c r="B200" s="20"/>
+      <c r="C200" s="21"/>
+      <c r="D200" s="6">
+        <v>8</v>
+      </c>
+      <c r="E200" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F200" s="8"/>
+      <c r="G200" s="9"/>
+      <c r="H200" s="18"/>
+      <c r="I200" s="22"/>
+    </row>
+    <row r="201" spans="1:11">
+      <c r="A201" s="19"/>
+      <c r="B201" s="20"/>
+      <c r="C201" s="21"/>
+      <c r="D201" s="6">
+        <v>9</v>
+      </c>
+      <c r="E201" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F201" s="8"/>
+      <c r="G201" s="9"/>
+      <c r="H201" s="18"/>
+      <c r="I201" s="22"/>
+    </row>
+    <row r="202" spans="1:11">
+      <c r="A202" s="19"/>
+      <c r="B202" s="20"/>
+      <c r="C202" s="21"/>
+      <c r="D202" s="6">
+        <v>10</v>
+      </c>
+      <c r="E202" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F202" s="8"/>
+      <c r="G202" s="9"/>
+      <c r="H202" s="18"/>
+      <c r="I202" s="22"/>
+      <c r="K202" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11">
+      <c r="A203" s="19"/>
+      <c r="B203" s="20"/>
+      <c r="C203" s="21"/>
+      <c r="D203" s="6">
+        <v>11</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F203" s="8"/>
+      <c r="G203" s="9"/>
+      <c r="H203" s="18"/>
+      <c r="I203" s="22"/>
+    </row>
+    <row r="204" spans="1:11">
+      <c r="A204" s="19"/>
+      <c r="B204" s="20"/>
+      <c r="C204" s="21"/>
+      <c r="D204" s="6">
+        <v>12</v>
+      </c>
+      <c r="E204" s="27" t="s">
+        <v>292</v>
+      </c>
+      <c r="F204" s="8"/>
+      <c r="G204" s="9"/>
+      <c r="H204" s="18"/>
+      <c r="I204" s="22"/>
+    </row>
+    <row r="205" spans="1:11">
+      <c r="A205" s="19"/>
+      <c r="B205" s="20"/>
+      <c r="C205" s="21"/>
+      <c r="D205" s="6">
+        <v>13</v>
+      </c>
+      <c r="E205" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F205" s="8"/>
+      <c r="G205" s="9"/>
+      <c r="H205" s="18"/>
+      <c r="I205" s="22"/>
+    </row>
+    <row r="206" spans="1:11">
+      <c r="A206" s="19"/>
+      <c r="B206" s="20"/>
+      <c r="C206" s="21"/>
+      <c r="D206" s="6">
+        <v>14</v>
+      </c>
+      <c r="E206" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F206" s="8"/>
+      <c r="G206" s="9"/>
+      <c r="H206" s="18"/>
+      <c r="I206" s="22"/>
+    </row>
+    <row r="207" spans="1:11">
+      <c r="A207" s="19"/>
+      <c r="B207" s="20"/>
+      <c r="C207" s="21"/>
+      <c r="D207" s="6">
+        <v>15</v>
+      </c>
+      <c r="E207" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F207" s="8"/>
+      <c r="G207" s="9"/>
+      <c r="H207" s="18"/>
+      <c r="I207" s="22"/>
+    </row>
+    <row r="208" spans="1:11">
+      <c r="A208" s="19"/>
+      <c r="B208" s="20"/>
+      <c r="C208" s="21"/>
+      <c r="D208" s="6">
+        <v>16</v>
+      </c>
+      <c r="E208" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F208" s="8"/>
+      <c r="G208" s="9"/>
+      <c r="H208" s="18"/>
+      <c r="I208" s="22"/>
+    </row>
+    <row r="209" spans="1:9">
+      <c r="A209" s="19"/>
+      <c r="B209" s="20"/>
+      <c r="C209" s="21"/>
+      <c r="D209" s="6">
+        <v>17</v>
+      </c>
+      <c r="E209" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F209" s="8"/>
+      <c r="G209" s="9"/>
+      <c r="H209" s="18"/>
+      <c r="I209" s="22"/>
+    </row>
+    <row r="210" spans="1:9">
+      <c r="A210" s="19"/>
+      <c r="B210" s="20"/>
+      <c r="C210" s="21"/>
+      <c r="D210" s="6">
+        <v>18</v>
+      </c>
+      <c r="E210" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F210" s="8"/>
+      <c r="G210" s="9"/>
+      <c r="H210" s="18"/>
+      <c r="I210" s="22"/>
+    </row>
+    <row r="211" spans="1:9">
+      <c r="A211" s="19"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="21"/>
+      <c r="D211" s="6">
+        <v>19</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F211" s="8"/>
+      <c r="G211" s="9"/>
+      <c r="H211" s="18"/>
+      <c r="I211" s="22"/>
+    </row>
+    <row r="212" spans="1:9">
+      <c r="A212" s="19"/>
+      <c r="B212" s="20"/>
+      <c r="C212" s="21"/>
+      <c r="D212" s="6">
+        <v>20</v>
+      </c>
+      <c r="E212" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F212" s="8"/>
+      <c r="G212" s="9"/>
+      <c r="H212" s="18"/>
+      <c r="I212" s="22"/>
+    </row>
+    <row r="213" spans="1:9">
+      <c r="A213" s="19"/>
+      <c r="B213" s="20"/>
+      <c r="C213" s="21"/>
+      <c r="D213" s="6">
+        <v>21</v>
+      </c>
+      <c r="E213" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F213" s="8"/>
+      <c r="G213" s="9"/>
+      <c r="H213" s="18"/>
+      <c r="I213" s="22"/>
+    </row>
+    <row r="214" spans="1:9">
+      <c r="A214" s="19"/>
+      <c r="B214" s="20"/>
+      <c r="C214" s="21"/>
+      <c r="D214" s="6">
+        <v>22</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F214" s="8"/>
+      <c r="G214" s="9"/>
+      <c r="H214" s="18"/>
+      <c r="I214" s="22"/>
+    </row>
+    <row r="215" spans="1:9">
+      <c r="A215" s="19"/>
+      <c r="B215" s="20"/>
+      <c r="C215" s="21"/>
+      <c r="D215" s="6">
+        <v>23</v>
+      </c>
+      <c r="E215" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="F215" s="8"/>
+      <c r="G215" s="9"/>
+      <c r="H215" s="18"/>
+      <c r="I215" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="89">
-    <mergeCell ref="A187:A188"/>
-    <mergeCell ref="B187:B188"/>
-    <mergeCell ref="C187:C188"/>
-    <mergeCell ref="I187:I188"/>
-    <mergeCell ref="A189:A192"/>
-    <mergeCell ref="B189:B192"/>
-    <mergeCell ref="C189:C192"/>
-    <mergeCell ref="I189:I192"/>
+  <mergeCells count="90">
+    <mergeCell ref="A193:A215"/>
+    <mergeCell ref="B193:B215"/>
+    <mergeCell ref="C193:C215"/>
+    <mergeCell ref="I193:I215"/>
+    <mergeCell ref="C187:C192"/>
+    <mergeCell ref="A187:A192"/>
+    <mergeCell ref="B187:B192"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:A23"/>
+    <mergeCell ref="B3:B23"/>
+    <mergeCell ref="C3:C23"/>
+    <mergeCell ref="I3:I19"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="B28:B35"/>
+    <mergeCell ref="C28:C35"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="A36:A41"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="I36:I41"/>
+    <mergeCell ref="A42:A47"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="C42:C47"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="A48:A59"/>
+    <mergeCell ref="B48:B59"/>
+    <mergeCell ref="C48:C59"/>
+    <mergeCell ref="I48:I59"/>
+    <mergeCell ref="A60:A66"/>
+    <mergeCell ref="B60:B66"/>
+    <mergeCell ref="C60:C66"/>
+    <mergeCell ref="I60:I66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="I67:I69"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="B70:B74"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="I70:I74"/>
+    <mergeCell ref="A75:A84"/>
+    <mergeCell ref="B75:B84"/>
+    <mergeCell ref="C75:C84"/>
+    <mergeCell ref="I75:I82"/>
+    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="C85:C88"/>
+    <mergeCell ref="I85:I88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="I92:I93"/>
+    <mergeCell ref="A94:A110"/>
+    <mergeCell ref="B94:B110"/>
+    <mergeCell ref="C94:C110"/>
+    <mergeCell ref="I94:I110"/>
+    <mergeCell ref="A111:A113"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="C111:C113"/>
+    <mergeCell ref="I111:I113"/>
+    <mergeCell ref="A114:A131"/>
+    <mergeCell ref="B114:B131"/>
+    <mergeCell ref="C114:C131"/>
+    <mergeCell ref="I115:I131"/>
     <mergeCell ref="A184:A186"/>
     <mergeCell ref="B184:B186"/>
     <mergeCell ref="C184:C186"/>
@@ -6334,185 +6819,122 @@
     <mergeCell ref="B182:B183"/>
     <mergeCell ref="C182:C183"/>
     <mergeCell ref="I182:I183"/>
-    <mergeCell ref="A111:A113"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="I111:I113"/>
-    <mergeCell ref="A114:A131"/>
-    <mergeCell ref="B114:B131"/>
-    <mergeCell ref="C114:C131"/>
-    <mergeCell ref="I115:I131"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="I92:I93"/>
-    <mergeCell ref="A94:A110"/>
-    <mergeCell ref="B94:B110"/>
-    <mergeCell ref="C94:C110"/>
-    <mergeCell ref="I94:I110"/>
-    <mergeCell ref="A85:A88"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="C85:C88"/>
-    <mergeCell ref="I85:I88"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="I89:I91"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="I70:I74"/>
-    <mergeCell ref="A75:A84"/>
-    <mergeCell ref="B75:B84"/>
-    <mergeCell ref="C75:C84"/>
-    <mergeCell ref="I75:I82"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="B60:B66"/>
-    <mergeCell ref="C60:C66"/>
-    <mergeCell ref="I60:I66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="I67:I69"/>
-    <mergeCell ref="A42:A47"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="C42:C47"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="A48:A59"/>
-    <mergeCell ref="B48:B59"/>
-    <mergeCell ref="C48:C59"/>
-    <mergeCell ref="I48:I59"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="B28:B35"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="I28:I35"/>
-    <mergeCell ref="A36:A41"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="C36:C41"/>
-    <mergeCell ref="I36:I41"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:A23"/>
-    <mergeCell ref="B3:B23"/>
-    <mergeCell ref="C3:C23"/>
-    <mergeCell ref="I3:I19"/>
+    <mergeCell ref="I187:I188"/>
+    <mergeCell ref="I189:I192"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="37" priority="37" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="38" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="duplicateValues" dxfId="36" priority="38" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="39" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="duplicateValues" dxfId="35" priority="4" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="5" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="duplicateValues" dxfId="34" priority="34" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="35" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="duplicateValues" dxfId="33" priority="18" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="19" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="duplicateValues" dxfId="32" priority="10" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="11" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="duplicateValues" dxfId="31" priority="33" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="34" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C99">
-    <cfRule type="duplicateValues" dxfId="30" priority="19" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="20" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100">
-    <cfRule type="duplicateValues" dxfId="29" priority="16" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="17" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
+    <cfRule type="duplicateValues" dxfId="29" priority="15" stopIfTrue="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
     <cfRule type="duplicateValues" dxfId="28" priority="14" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
-    <cfRule type="duplicateValues" dxfId="27" priority="13" stopIfTrue="1"/>
+  <conditionalFormatting sqref="C105">
+    <cfRule type="duplicateValues" dxfId="27" priority="10" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
+  <conditionalFormatting sqref="C106">
     <cfRule type="duplicateValues" dxfId="26" priority="9" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
+  <conditionalFormatting sqref="C107">
     <cfRule type="duplicateValues" dxfId="25" priority="8" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="duplicateValues" dxfId="24" priority="7" stopIfTrue="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C110">
-    <cfRule type="duplicateValues" dxfId="23" priority="5" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="6" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114">
-    <cfRule type="duplicateValues" dxfId="22" priority="23" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="24" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C178">
-    <cfRule type="duplicateValues" dxfId="21" priority="17" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="18" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C180">
-    <cfRule type="duplicateValues" dxfId="20" priority="20" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="21" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C182">
-    <cfRule type="duplicateValues" dxfId="19" priority="15" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="16" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C184">
-    <cfRule type="duplicateValues" dxfId="18" priority="12" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="13" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="duplicateValues" dxfId="17" priority="39" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="40" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="duplicateValues" dxfId="16" priority="35" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="36" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C35">
-    <cfRule type="duplicateValues" dxfId="15" priority="36" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="37" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C41">
+    <cfRule type="duplicateValues" dxfId="15" priority="31" stopIfTrue="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67:C69">
     <cfRule type="duplicateValues" dxfId="14" priority="30" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C67:C69">
+  <conditionalFormatting sqref="C70:C74">
     <cfRule type="duplicateValues" dxfId="13" priority="29" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C74">
+  <conditionalFormatting sqref="C85:C88">
     <cfRule type="duplicateValues" dxfId="12" priority="28" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85:C88">
+  <conditionalFormatting sqref="C89:C91">
     <cfRule type="duplicateValues" dxfId="11" priority="27" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89:C91">
+  <conditionalFormatting sqref="C92:C93">
     <cfRule type="duplicateValues" dxfId="10" priority="26" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C92:C93">
-    <cfRule type="duplicateValues" dxfId="9" priority="25" stopIfTrue="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C96:C98">
-    <cfRule type="duplicateValues" dxfId="8" priority="22" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="23" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C103:C104">
-    <cfRule type="duplicateValues" dxfId="7" priority="11" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108:C109">
-    <cfRule type="duplicateValues" dxfId="6" priority="6" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:C45 C47">
-    <cfRule type="duplicateValues" dxfId="5" priority="31" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="32" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C63 C66">
-    <cfRule type="duplicateValues" dxfId="4" priority="32" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="33" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111:C113 C94:C95">
-    <cfRule type="duplicateValues" dxfId="3" priority="24" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="25" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C132:C177 C179">
-    <cfRule type="duplicateValues" dxfId="2" priority="21" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="22" stopIfTrue="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C187">
-    <cfRule type="duplicateValues" dxfId="1" priority="2" stopIfTrue="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C189:C191">
+  <conditionalFormatting sqref="C193:C214">
     <cfRule type="duplicateValues" dxfId="0" priority="1" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>